<commit_message>
MDO bulk approval default fields file
</commit_message>
<xml_diff>
--- a/MDO/client-assets/assets/common/user-approvals-upload-sample.xlsx
+++ b/MDO/client-assets/assets/common/user-approvals-upload-sample.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{937AFDF7-6D64-41CB-ADF8-3306C34C0993}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sureshkannan\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46A58F6-B166-493C-BAA3-669381F28A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,50 +68,50 @@
     <t>Location</t>
   </si>
   <si>
-    <t>usershankar@yopmail.com</t>
-  </si>
-  <si>
     <t>Railway Protection Service</t>
   </si>
   <si>
-    <t>shankarusr1@yopmail.com</t>
-  </si>
-  <si>
-    <t>usernarayan@yopmail.com</t>
-  </si>
-  <si>
     <t>Healthcare</t>
   </si>
   <si>
-    <t>usershankar001@yopmail.com</t>
-  </si>
-  <si>
     <t>Indian Cost Accounts Service</t>
   </si>
   <si>
-    <t>usershankar002@yopmail.com</t>
-  </si>
-  <si>
     <t>CHIEF MEDIA</t>
   </si>
   <si>
     <t>Central Health Service</t>
   </si>
   <si>
-    <t>useradarsh@yopmail.com</t>
-  </si>
-  <si>
     <t>Group A</t>
   </si>
   <si>
     <t>Mauritius</t>
+  </si>
+  <si>
+    <t>new_user01@yopmail.com</t>
+  </si>
+  <si>
+    <t>new_user02@yopmail.com</t>
+  </si>
+  <si>
+    <t>new_user03@yopmail.com</t>
+  </si>
+  <si>
+    <t>new_user04@yopmail.com</t>
+  </si>
+  <si>
+    <t>new_user05@yopmail.com</t>
+  </si>
+  <si>
+    <t>new_user06@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,23 +491,23 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,89 +539,90 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>9922222222</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
-        <v>7259895669</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3">
-        <v>9864534414</v>
+        <v>8520222222</v>
       </c>
       <c r="H3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>7682613245</v>
+        <v>8522222333</v>
       </c>
       <c r="C4" s="2">
         <v>37044</v>
       </c>
       <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>9788555555</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>9555522222</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>9555222222</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>9724355691</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="J7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>6758365253</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <v>8836745262</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{3C3005BB-4FE7-43E7-A3D5-FF83208372B0}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{D329D20B-385E-468C-A5EA-A6DA496C79B3}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{38457610-1447-4478-8C2E-6ACB5B9ABD9C}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{E935224A-C0A8-4974-8C36-75F08B6EB838}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{F8D0F605-AE2C-468D-A1E7-E2CEA2D3AB52}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{EDABD25E-D7E7-457E-BA5E-2C323899C8CA}"/>
+    <hyperlink ref="A3:A7" r:id="rId2" display="new_user01@yopmail.com" xr:uid="{7C95973B-4174-4B0D-9400-374FCD667648}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{59F00B1D-7139-4FC4-BF35-10DDCC7FAB8A}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{C038AC3B-C7B7-4C36-9B11-2D488B755B54}"/>
+    <hyperlink ref="A5" r:id="rId5" xr:uid="{8F6B271A-5FBA-4F65-B02C-2B9F8C875A37}"/>
+    <hyperlink ref="A6" r:id="rId6" xr:uid="{23D0DFED-F2F8-4E9E-B9BE-0256B3105BAA}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{56A22BF3-8D5F-4ED2-9B89-CF90F3C3C0AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>